<commit_message>
Asignación de autores recursos en greco Mat 9 tema 6
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion06/ESCALETA_MA_09_06_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion06/ESCALETA_MA_09_06_CO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Documents\GitHub\Matematicas\fuentes\contenidos\grado09\guion06\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
@@ -10,12 +15,12 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="297">
   <si>
     <t>Asignatura</t>
   </si>
@@ -885,6 +890,30 @@
   </si>
   <si>
     <t>m101ap</t>
+  </si>
+  <si>
+    <t>Autores</t>
+  </si>
+  <si>
+    <t>Johanna Montejo</t>
+  </si>
+  <si>
+    <t>Jairo Saavedra</t>
+  </si>
+  <si>
+    <t>Magda González</t>
+  </si>
+  <si>
+    <t>Adriana Lasprilla</t>
+  </si>
+  <si>
+    <t>Jennifer Rojas</t>
+  </si>
+  <si>
+    <t>Jaennifer Rojas</t>
+  </si>
+  <si>
+    <t>Andrea Santos</t>
   </si>
 </sst>
 </file>
@@ -1208,15 +1237,6 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1260,6 +1280,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1322,7 +1351,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1357,7 +1386,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1566,10 +1595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U181"/>
+  <dimension ref="A1:V181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="T45" sqref="T45"/>
+    <sheetView tabSelected="1" topLeftCell="H14" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1588,92 +1617,95 @@
     <col min="12" max="12" width="15.140625" style="12" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.28515625" style="12" customWidth="1"/>
     <col min="14" max="14" width="14.7109375" style="12" customWidth="1"/>
-    <col min="15" max="15" width="56" style="12" customWidth="1"/>
-    <col min="16" max="16" width="17.5703125" style="12" customWidth="1"/>
-    <col min="17" max="17" width="16.140625" style="32" customWidth="1"/>
-    <col min="18" max="18" width="10" style="32" customWidth="1"/>
-    <col min="19" max="19" width="14.7109375" style="32" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="23" style="32" customWidth="1"/>
-    <col min="21" max="21" width="15" style="32" customWidth="1"/>
+    <col min="15" max="15" width="56" style="12" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="17.5703125" style="12" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="16.140625" style="32" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="10" style="32" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="14.7109375" style="32" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="23" style="32" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="15" style="32" hidden="1" customWidth="1"/>
     <col min="22" max="16384" width="11.42578125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="14" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:22" s="14" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="48" t="s">
         <v>219</v>
       </c>
-      <c r="E1" s="53" t="s">
+      <c r="E1" s="50" t="s">
         <v>220</v>
       </c>
-      <c r="F1" s="51" t="s">
+      <c r="F1" s="48" t="s">
         <v>221</v>
       </c>
-      <c r="G1" s="42" t="s">
+      <c r="G1" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="47" t="s">
+      <c r="H1" s="44" t="s">
         <v>216</v>
       </c>
-      <c r="I1" s="49" t="s">
+      <c r="I1" s="46" t="s">
         <v>113</v>
       </c>
-      <c r="J1" s="44" t="s">
+      <c r="J1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="43" t="s">
+      <c r="K1" s="40" t="s">
         <v>217</v>
       </c>
-      <c r="L1" s="42" t="s">
+      <c r="L1" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="45" t="s">
+      <c r="M1" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="45"/>
+      <c r="N1" s="42"/>
       <c r="O1" s="36" t="s">
         <v>112</v>
       </c>
       <c r="P1" s="36" t="s">
         <v>218</v>
       </c>
-      <c r="Q1" s="37" t="s">
+      <c r="Q1" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="R1" s="39" t="s">
+      <c r="R1" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="S1" s="37" t="s">
+      <c r="S1" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="T1" s="38" t="s">
+      <c r="T1" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="U1" s="37" t="s">
+      <c r="U1" s="52" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" s="14" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="41"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="42"/>
+      <c r="V1" s="14" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" s="14" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="38"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="39"/>
       <c r="M2" s="13" t="s">
         <v>40</v>
       </c>
@@ -1682,13 +1714,13 @@
       </c>
       <c r="O2" s="36"/>
       <c r="P2" s="36"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="39"/>
-      <c r="S2" s="37"/>
-      <c r="T2" s="38"/>
-      <c r="U2" s="37"/>
-    </row>
-    <row r="3" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q2" s="52"/>
+      <c r="R2" s="54"/>
+      <c r="S2" s="52"/>
+      <c r="T2" s="53"/>
+      <c r="U2" s="52"/>
+    </row>
+    <row r="3" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -1746,8 +1778,11 @@
       <c r="U3" s="28" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V3" s="12" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1807,8 +1842,11 @@
       <c r="U4" s="28" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V4" s="12" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1866,8 +1904,11 @@
       <c r="U5" s="28" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V5" s="12" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1924,7 +1965,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1982,8 +2023,11 @@
       <c r="U7" s="28" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V7" s="12" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -2043,8 +2087,11 @@
       <c r="U8" s="28" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V8" s="12" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -2102,8 +2149,11 @@
       <c r="U9" s="28" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V9" s="12" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -2161,8 +2211,11 @@
       <c r="U10" s="28" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="11" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V10" s="12" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -2221,7 +2274,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -2280,7 +2333,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -2339,7 +2392,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
@@ -2399,8 +2452,11 @@
       <c r="U14" s="28" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V14" s="12" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
@@ -2460,8 +2516,11 @@
       <c r="U15" s="28" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="16" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V15" s="12" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
@@ -2520,7 +2579,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
@@ -2578,8 +2637,11 @@
       <c r="U17" s="28" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="18" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V17" s="12" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
@@ -2637,8 +2699,11 @@
       <c r="U18" s="28" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="19" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V18" s="12" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>8</v>
       </c>
@@ -2696,8 +2761,11 @@
       <c r="U19" s="28" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V19" s="12" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
@@ -2757,8 +2825,11 @@
       <c r="U20" s="28" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V20" s="12" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>8</v>
       </c>
@@ -2820,8 +2891,11 @@
       <c r="U21" s="28" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V21" s="12" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>8</v>
       </c>
@@ -2883,8 +2957,11 @@
       <c r="U22" s="28" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="23" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V22" s="12" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>8</v>
       </c>
@@ -2942,8 +3019,11 @@
       <c r="U23" s="28" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V23" s="12" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>8</v>
       </c>
@@ -3001,8 +3081,11 @@
       <c r="U24" s="28" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="25" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V24" s="12" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>8</v>
       </c>
@@ -3062,8 +3145,11 @@
       <c r="U25" s="28" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="26" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V25" s="12" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>8</v>
       </c>
@@ -3123,8 +3209,11 @@
       <c r="U26" s="28" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="27" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V26" s="12" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>8</v>
       </c>
@@ -3182,8 +3271,11 @@
       <c r="U27" s="28" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="28" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V27" s="12" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>8</v>
       </c>
@@ -3241,8 +3333,11 @@
       <c r="U28" s="28" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="29" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V28" s="12" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>8</v>
       </c>
@@ -3302,8 +3397,11 @@
       <c r="U29" s="28" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="30" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V29" s="12" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>8</v>
       </c>
@@ -3363,8 +3461,11 @@
       <c r="U30" s="28" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="31" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V30" s="12" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>8</v>
       </c>
@@ -3424,8 +3525,11 @@
       <c r="U31" s="28" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="32" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V31" s="12" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>8</v>
       </c>
@@ -3483,8 +3587,11 @@
       <c r="U32" s="28" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="33" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V32" s="12" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>8</v>
       </c>
@@ -3544,8 +3651,11 @@
       <c r="U33" s="28" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="34" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V33" s="12" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>8</v>
       </c>
@@ -3605,8 +3715,11 @@
       <c r="U34" s="28" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="35" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V34" s="12" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>8</v>
       </c>
@@ -3666,8 +3779,11 @@
       <c r="U35" s="28" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="36" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V35" s="12" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>8</v>
       </c>
@@ -3724,7 +3840,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="37" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>8</v>
       </c>
@@ -3761,7 +3877,7 @@
       <c r="T37" s="31"/>
       <c r="U37" s="28"/>
     </row>
-    <row r="38" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>8</v>
       </c>
@@ -3821,8 +3937,11 @@
       <c r="U38" s="28" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="39" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V38" s="12" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>8</v>
       </c>
@@ -3876,23 +3995,26 @@
       <c r="U39" s="28" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="40" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V39" s="12" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G40" s="33"/>
       <c r="H40" s="34"/>
       <c r="I40" s="33"/>
     </row>
-    <row r="41" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G41" s="33"/>
       <c r="H41" s="35"/>
       <c r="I41" s="33"/>
     </row>
-    <row r="42" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G42" s="33"/>
       <c r="H42" s="34"/>
       <c r="I42" s="33"/>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="G43" s="33"/>
       <c r="H43" s="33"/>
       <c r="I43" s="33"/>
@@ -4658,6 +4780,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
@@ -4672,12 +4800,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P3">

</xml_diff>

<commit_message>
Asignación de autores de at 9 tema 6
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion06/ESCALETA_MA_09_06_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion06/ESCALETA_MA_09_06_CO.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="296">
   <si>
     <t>Asignatura</t>
   </si>
@@ -908,9 +908,6 @@
   </si>
   <si>
     <t>Jennifer Rojas</t>
-  </si>
-  <si>
-    <t>Jaennifer Rojas</t>
   </si>
   <si>
     <t>Andrea Santos</t>
@@ -1597,8 +1594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H14" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+    <sheetView tabSelected="1" topLeftCell="H17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2958,7 +2955,7 @@
         <v>199</v>
       </c>
       <c r="V22" s="12" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="23" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -3146,7 +3143,7 @@
         <v>199</v>
       </c>
       <c r="V25" s="12" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="26" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -3272,7 +3269,7 @@
         <v>193</v>
       </c>
       <c r="V27" s="12" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="28" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -3334,7 +3331,7 @@
         <v>199</v>
       </c>
       <c r="V28" s="12" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="29" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -3398,7 +3395,7 @@
         <v>199</v>
       </c>
       <c r="V29" s="12" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="30" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -3462,7 +3459,7 @@
         <v>199</v>
       </c>
       <c r="V30" s="12" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="31" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -3526,7 +3523,7 @@
         <v>199</v>
       </c>
       <c r="V31" s="12" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="32" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -3588,7 +3585,7 @@
         <v>199</v>
       </c>
       <c r="V32" s="12" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="33" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -3652,7 +3649,7 @@
         <v>199</v>
       </c>
       <c r="V33" s="12" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="34" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Revert "Asignación de autores de at 9 tema 6"
This reverts commit adde3fef94ee4bb02cd7bb2c8287dc4fa3339b4e.
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion06/ESCALETA_MA_09_06_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion06/ESCALETA_MA_09_06_CO.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="297">
   <si>
     <t>Asignatura</t>
   </si>
@@ -908,6 +908,9 @@
   </si>
   <si>
     <t>Jennifer Rojas</t>
+  </si>
+  <si>
+    <t>Jaennifer Rojas</t>
   </si>
   <si>
     <t>Andrea Santos</t>
@@ -1594,8 +1597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H17" sqref="A17:XFD17"/>
+    <sheetView tabSelected="1" topLeftCell="H14" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2955,7 +2958,7 @@
         <v>199</v>
       </c>
       <c r="V22" s="12" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="23" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -3143,7 +3146,7 @@
         <v>199</v>
       </c>
       <c r="V25" s="12" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="26" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -3269,7 +3272,7 @@
         <v>193</v>
       </c>
       <c r="V27" s="12" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="28" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -3331,7 +3334,7 @@
         <v>199</v>
       </c>
       <c r="V28" s="12" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="29" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -3395,7 +3398,7 @@
         <v>199</v>
       </c>
       <c r="V29" s="12" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="30" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -3459,7 +3462,7 @@
         <v>199</v>
       </c>
       <c r="V30" s="12" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="31" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -3523,7 +3526,7 @@
         <v>199</v>
       </c>
       <c r="V31" s="12" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="32" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -3585,7 +3588,7 @@
         <v>199</v>
       </c>
       <c r="V32" s="12" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="33" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
@@ -3649,7 +3652,7 @@
         <v>199</v>
       </c>
       <c r="V33" s="12" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="34" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>